<commit_message>
add some carter tests
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/searchItems.xlsx
+++ b/src/test/resources/testData/searchItems.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohannadhussein/Desktop/MohannadWorkSpace/TestNGMavenProject/src/test/resources/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0AA9FA2-F9B9-A447-998E-89FFE6E336E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5DE246-E2F0-D548-B90B-4B0C437B0256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16360" xr2:uid="{C1F361A3-8ADB-F147-8B91-8258C64E132F}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16340" xr2:uid="{C1F361A3-8ADB-F147-8B91-8258C64E132F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
-    <t>coffee mug</t>
-  </si>
-  <si>
     <t>pretty coffee mug</t>
   </si>
   <si>
@@ -69,6 +66,9 @@
   </si>
   <si>
     <t>Search Items</t>
+  </si>
+  <si>
+    <t>Aleheida</t>
   </si>
 </sst>
 </file>
@@ -137,7 +137,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -425,7 +425,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -436,7 +436,7 @@
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -446,57 +446,57 @@
   <sheetData>
     <row r="1" spans="1:1" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>